<commit_message>
Changed out barrel jack. Still needs to be connected to ground. I think there's an issue with the footprint. Also rounded the edges of the board.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20377"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20378"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nas01.itap.purdue.edu\puhome\My Documents\PIANO-PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2CD6555E-3DD0-4B76-BD65-0D2D2DCCDE69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607168D4-17D3-4AC3-B3B7-9DF7D99EA786}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{9C341551-46EE-4913-BBAA-A2934560D97C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Quantity</t>
   </si>
@@ -105,12 +105,6 @@
     <t>Terminal Block Connector</t>
   </si>
   <si>
-    <t>RESET C</t>
-  </si>
-  <si>
-    <t>TODO</t>
-  </si>
-  <si>
     <t>Currently Have</t>
   </si>
   <si>
@@ -151,13 +145,31 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/sullins-connector-solutions/PPTC071LFBN-RC/810146</t>
+  </si>
+  <si>
+    <t>Lab</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>50kΩ Resistor 0805</t>
+  </si>
+  <si>
+    <t>0.01µF Capacitor 0805</t>
+  </si>
+  <si>
+    <t>On List</t>
+  </si>
+  <si>
+    <t>Already Have</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,16 +193,65 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -198,19 +259,62 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="5"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="6">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Input" xfId="4" builtinId="20"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="5" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -522,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FA0834F-0348-4DB4-AEB9-16BE25F3E166}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,13 +649,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -564,7 +668,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B2">
@@ -574,24 +678,24 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F2">
         <v>0.84</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G23" si="0">F2*B2</f>
+        <f t="shared" ref="G2:G25" si="0">F2*B2</f>
         <v>0.84</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B3">
@@ -603,7 +707,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B4">
@@ -613,10 +717,10 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F4">
         <v>0.33</v>
@@ -626,15 +730,15 @@
         <v>0.33</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
@@ -642,7 +746,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B6">
@@ -654,7 +758,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B7">
@@ -666,241 +770,277 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>3</v>
       </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B12">
+      <c r="B14">
         <v>4</v>
       </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
         <v>317030213</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
         <v>317030213</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20">
+        <v>9.9</v>
+      </c>
+      <c r="G20">
+        <f>F20*B20</f>
+        <v>9.9</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="F18">
-        <v>9.9</v>
-      </c>
-      <c r="G18">
-        <f>F18*B18</f>
-        <v>9.9</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20">
-        <v>0.59</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="0"/>
-        <v>0.59</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22">
+        <v>0.59</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>0.59</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" t="s">
-        <v>27</v>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" xr:uid="{DC6C5664-1C22-41A0-AB9F-3C0E9C06A62D}"/>
     <hyperlink ref="H4" r:id="rId2" xr:uid="{1328E90D-5A53-4E80-B13A-9AED72B43FEB}"/>
-    <hyperlink ref="H18" r:id="rId3" xr:uid="{6ACE24BB-F3BB-4905-AFA9-2FC4986FB4DA}"/>
-    <hyperlink ref="H20" r:id="rId4" xr:uid="{73E2C549-E9E5-423F-B4A8-3D110E314A06}"/>
+    <hyperlink ref="H20" r:id="rId3" xr:uid="{6ACE24BB-F3BB-4905-AFA9-2FC4986FB4DA}"/>
+    <hyperlink ref="H22" r:id="rId4" xr:uid="{73E2C549-E9E5-423F-B4A8-3D110E314A06}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId5"/>

</xml_diff>